<commit_message>
project folder cleanup src.py cleanup
</commit_message>
<xml_diff>
--- a/src/input/00 Client information.xlsx
+++ b/src/input/00 Client information.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="588" yWindow="576" windowWidth="15996" windowHeight="6564"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Info" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Existing Insurance" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Beneficiaries" sheetId="3" r:id="rId6"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing Insurance" sheetId="2" r:id="rId2"/>
+    <sheet name="Beneficiaries" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t>POLICY NUMBER</t>
   </si>
@@ -132,9 +135,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>HKID</t>
-  </si>
-  <si>
     <t>DATE OF BIRTH (DD/MM/YY)</t>
   </si>
   <si>
@@ -189,12 +189,6 @@
     <t>AREA CODE</t>
   </si>
   <si>
-    <t>RESIDENTIAL NUMBER</t>
-  </si>
-  <si>
-    <t>OFFICE NUMBER</t>
-  </si>
-  <si>
     <t>HOUSE/APT/SUITE/NUMBER/STREET</t>
   </si>
   <si>
@@ -334,36 +328,53 @@
   </si>
   <si>
     <t>INVESTMENT VALUE (MUTUAL FUNDS / UNIT TRUSTS)</t>
+  </si>
+  <si>
+    <t>HKID OR PASSPORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font/>
-    <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -371,7 +382,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -381,67 +392,54 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -631,644 +629,629 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.75"/>
-    <col customWidth="1" min="2" max="2" width="67.63"/>
-    <col customWidth="1" min="3" max="3" width="8.5"/>
-    <col customWidth="1" min="4" max="4" width="32.5"/>
-    <col customWidth="1" min="5" max="5" width="9.0"/>
-    <col customWidth="1" min="6" max="6" width="11.25"/>
-    <col customWidth="1" min="7" max="26" width="7.63"/>
+    <col min="1" max="1" width="41.69921875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="67.59765625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" style="9" customWidth="1"/>
+    <col min="7" max="26" width="7.59765625" style="9" customWidth="1"/>
+    <col min="27" max="16384" width="12.59765625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
-        <v>6.11067085E8</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="B1" s="8">
+        <v>611067085</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="11">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="10" t="s">
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="11">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="11">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="11">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="11">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="11">
+        <v>553595566</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="6">
-        <v>5.53595566E8</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="11">
+        <v>971</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="6">
-        <v>971.0</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="11">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="10" t="s">
+      <c r="B25" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="10" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="B26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="6" t="s">
+      <c r="B27" s="11">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A29" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="6" t="s">
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="6" t="s">
+      <c r="B31" s="11">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A32" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="11">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="10" t="s">
+    </row>
+    <row r="33" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="8" t="s">
+      <c r="B33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A34" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="B34" s="11">
+        <v>0</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A35" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="8" t="s">
+      <c r="B35" s="11">
+        <v>0</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="36" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A36" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="10" t="s">
+      <c r="B36" s="11">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10" t="s">
+    </row>
+    <row r="37" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A37" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="10" t="s">
+      <c r="B37" s="11">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A38" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10" t="s">
+      <c r="B38" s="11">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A39" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="10" t="s">
+      <c r="B39" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="8">
-        <v>0.0</v>
-      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="10" t="s">
+    <row r="41" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7"/>
+    </row>
+    <row r="42" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A42" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A43" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="9" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A44" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
-      <c r="X43" s="9"/>
-      <c r="Y43" s="9"/>
-      <c r="Z43" s="9"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="9" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A45" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="9" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="9" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="9" t="s">
+    </row>
+    <row r="47" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A47" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="9" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
+    </row>
+    <row r="48" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A48" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="9" t="s">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A49" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="9" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A50" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="9" t="s">
+    <row r="51" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A51" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="9" t="s">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A52" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="9" t="s">
+    <row r="53" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A53" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="9" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A54" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9" t="s">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A55" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="9" t="s">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="9" t="s">
+    </row>
+    <row r="56" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A56" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="9" t="s">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A57" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A58" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2228,86 +2211,80 @@
     <row r="1021" ht="14.25" customHeight="1"/>
     <row r="1022" ht="14.25" customHeight="1"/>
     <row r="1023" ht="14.25" customHeight="1"/>
-    <row r="1024" ht="14.25" customHeight="1"/>
-    <row r="1025" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.5"/>
-    <col customWidth="1" min="2" max="2" width="16.25"/>
-    <col customWidth="1" min="3" max="3" width="8.38"/>
-    <col customWidth="1" min="4" max="4" width="4.38"/>
-    <col customWidth="1" min="5" max="5" width="8.88"/>
-    <col customWidth="1" min="6" max="6" width="11.13"/>
-    <col customWidth="1" min="7" max="7" width="10.13"/>
-    <col customWidth="1" min="8" max="26" width="7.63"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" customWidth="1"/>
+    <col min="6" max="6" width="11.09765625" customWidth="1"/>
+    <col min="7" max="7" width="10.09765625" customWidth="1"/>
+    <col min="8" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1">
       <c r="A2" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1">
       <c r="A4" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3293,52 +3270,48 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.13"/>
-    <col customWidth="1" min="2" max="2" width="19.0"/>
-    <col customWidth="1" min="3" max="3" width="19.88"/>
-    <col customWidth="1" min="4" max="4" width="26.13"/>
-    <col customWidth="1" min="5" max="5" width="13.75"/>
-    <col customWidth="1" min="6" max="27" width="7.63"/>
+    <col min="1" max="1" width="13.09765625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" customWidth="1"/>
+    <col min="4" max="4" width="26.09765625" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" customWidth="1"/>
+    <col min="6" max="27" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>6.11067085E8</v>
+        <v>611067085</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -3348,29 +3321,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1">
       <c r="A4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -3388,9 +3361,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:6" ht="14.25" customHeight="1">
       <c r="A5" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -3408,17 +3381,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4405,9 +4378,7 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more forms in templates.json and change some fields in excel file
</commit_message>
<xml_diff>
--- a/src/input/00 Client information.xlsx
+++ b/src/input/00 Client information.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="588" yWindow="576" windowWidth="15996" windowHeight="6564"/>
-  </bookViews>
   <sheets>
-    <sheet name="Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Existing Insurance" sheetId="2" r:id="rId2"/>
-    <sheet name="Beneficiaries" sheetId="3" r:id="rId3"/>
+    <sheet state="visible" name="Info" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Existing Insurance" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Beneficiaries" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+  <si>
+    <t>No.</t>
+  </si>
   <si>
     <t>POLICY NUMBER</t>
   </si>
   <si>
-    <t>No.</t>
+    <t>OWNER OR INSURED</t>
   </si>
   <si>
     <t>NAME</t>
@@ -30,6 +30,21 @@
     <t>RELATIONSHIP TO SETTLOR</t>
   </si>
   <si>
+    <t>COMPANY</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>CURRENCY</t>
+  </si>
+  <si>
+    <t>SUM INSURED</t>
+  </si>
+  <si>
+    <t>ISSUED YEAR</t>
+  </si>
+  <si>
     <t>RELATIONSHIP TO LIFE INSURED</t>
   </si>
   <si>
@@ -45,13 +60,13 @@
     <t>self</t>
   </si>
   <si>
+    <t>Client Information</t>
+  </si>
+  <si>
     <t>B5881192</t>
   </si>
   <si>
-    <t>OWNER OR INSURED</t>
-  </si>
-  <si>
-    <t>Client Information</t>
+    <t>INSURED</t>
   </si>
   <si>
     <t>a</t>
@@ -63,6 +78,9 @@
     <t>c</t>
   </si>
   <si>
+    <t>OWNER</t>
+  </si>
+  <si>
     <t>d</t>
   </si>
   <si>
@@ -78,36 +96,21 @@
     <t>h</t>
   </si>
   <si>
-    <t>INSURED</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
     <t>f</t>
   </si>
   <si>
-    <t>COMPANY</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
-    <t>SUM INSURED</t>
-  </si>
-  <si>
-    <t>ISSUED YEAR</t>
-  </si>
-  <si>
-    <t>OWNER</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
     <t>FAMILY NAME</t>
   </si>
   <si>
@@ -135,6 +138,9 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>HKID</t>
+  </si>
+  <si>
     <t>DATE OF BIRTH (DD/MM/YY)</t>
   </si>
   <si>
@@ -189,6 +195,12 @@
     <t>AREA CODE</t>
   </si>
   <si>
+    <t>RESIDENTIAL NUMBER</t>
+  </si>
+  <si>
+    <t>OFFICE NUMBER</t>
+  </si>
+  <si>
     <t>HOUSE/APT/SUITE/NUMBER/STREET</t>
   </si>
   <si>
@@ -204,7 +216,7 @@
     <t>STATE/PROVINCE</t>
   </si>
   <si>
-    <t xml:space="preserve">COUNTRY </t>
+    <t>COUNTRY</t>
   </si>
   <si>
     <t>UAE</t>
@@ -328,53 +340,36 @@
   </si>
   <si>
     <t>INVESTMENT VALUE (MUTUAL FUNDS / UNIT TRUSTS)</t>
-  </si>
-  <si>
-    <t>HKID OR PASSPORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -382,7 +377,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -392,54 +387,67 @@
     </fill>
   </fills>
   <borders count="2">
+    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="11">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -629,629 +637,653 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1023"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="41.69921875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="67.59765625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="9" customWidth="1"/>
-    <col min="4" max="4" width="32.5" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.19921875" style="9" customWidth="1"/>
-    <col min="7" max="26" width="7.59765625" style="9" customWidth="1"/>
-    <col min="27" max="16384" width="12.59765625" style="9"/>
+    <col customWidth="1" min="1" max="1" width="41.75"/>
+    <col customWidth="1" min="2" max="2" width="67.63"/>
+    <col customWidth="1" min="3" max="3" width="8.5"/>
+    <col customWidth="1" min="4" max="4" width="32.5"/>
+    <col customWidth="1" min="5" max="5" width="9.0"/>
+    <col customWidth="1" min="6" max="6" width="11.25"/>
+    <col customWidth="1" min="7" max="26" width="7.63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8">
-        <v>611067085</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="8" t="s">
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4">
+        <v>6.11067085E8</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A4" s="11" t="s">
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="11">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A13" s="11" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="11">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="11">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="B13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="11">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="B14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="11">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A18" s="11" t="s">
+      <c r="B15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="11">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="B16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" s="11" t="s">
+      <c r="B18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="11">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="B19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="11">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="B20" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="11">
-        <v>553595566</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="11">
-        <v>971</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="B21" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="11">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="B22" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B23" s="7">
+        <v>5.53595566E8</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="B24" s="7">
+        <v>971.0</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B25" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="B26" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="11">
-        <v>0</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" s="11" t="s">
+      <c r="B27" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A29" s="11" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="11">
-        <v>0</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="11" t="s">
+      <c r="B29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="B30" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="11">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A32" s="11" t="s">
+      <c r="B31" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="11">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="B32" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="11">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A34" s="11" t="s">
+      <c r="B33" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="11">
-        <v>0</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="11">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B35" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="11">
-        <v>0</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A37" s="8" t="s">
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="11">
-        <v>0</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A38" s="8" t="s">
+      <c r="B37" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="11">
-        <v>0</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A39" s="8" t="s">
+      <c r="B38" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="11" t="s">
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
+      <c r="B39" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="A40" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0.0</v>
+      </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A41" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="7"/>
-      <c r="V41" s="7"/>
-      <c r="W41" s="7"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="7"/>
-      <c r="Z41" s="7"/>
-    </row>
-    <row r="42" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A42" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A43" s="7" t="s">
+    <row r="41" ht="14.25" customHeight="1">
+      <c r="A41" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A44" s="7" t="s">
+      <c r="B41" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="A42" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A45" s="7" t="s">
+      <c r="B42" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A46" s="7" t="s">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7" t="s">
+      <c r="B44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A47" s="7" t="s">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="A46" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="A47" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A48" s="7" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7" t="s">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A49" s="7" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A50" s="7" t="s">
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7" t="s">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A51" s="7" t="s">
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A52" s="7" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7" t="s">
+    </row>
+    <row r="52" ht="14.25" customHeight="1">
+      <c r="A52" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A53" s="7" t="s">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A54" s="7" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A55" s="7" t="s">
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="A54" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7" t="s">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" ht="14.25" customHeight="1">
+      <c r="A55" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A56" s="7" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A57" s="7" t="s">
+    </row>
+    <row r="56" ht="14.25" customHeight="1">
+      <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A58" s="7" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" ht="14.25" customHeight="1">
+      <c r="A57" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:4" ht="14.25" customHeight="1"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" ht="14.25" customHeight="1">
+      <c r="A58" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" ht="14.25" customHeight="1">
+      <c r="A59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" ht="14.25" customHeight="1">
+      <c r="A60" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2211,80 +2243,87 @@
     <row r="1021" ht="14.25" customHeight="1"/>
     <row r="1022" ht="14.25" customHeight="1"/>
     <row r="1023" ht="14.25" customHeight="1"/>
+    <row r="1024" ht="14.25" customHeight="1"/>
+    <row r="1025" ht="14.25" customHeight="1"/>
+    <row r="1026" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
-    <col min="3" max="3" width="8.3984375" customWidth="1"/>
-    <col min="4" max="4" width="4.3984375" customWidth="1"/>
-    <col min="5" max="5" width="8.8984375" customWidth="1"/>
-    <col min="6" max="6" width="11.09765625" customWidth="1"/>
-    <col min="7" max="7" width="10.09765625" customWidth="1"/>
-    <col min="8" max="26" width="7.59765625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="3.5"/>
+    <col customWidth="1" min="2" max="2" width="16.25"/>
+    <col customWidth="1" min="3" max="3" width="8.38"/>
+    <col customWidth="1" min="4" max="4" width="4.38"/>
+    <col customWidth="1" min="5" max="5" width="8.88"/>
+    <col customWidth="1" min="6" max="6" width="11.13"/>
+    <col customWidth="1" min="7" max="7" width="10.13"/>
+    <col customWidth="1" min="8" max="26" width="7.63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A3" s="2">
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1"/>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3270,128 +3309,132 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1001"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="19.8984375" customWidth="1"/>
-    <col min="4" max="4" width="26.09765625" customWidth="1"/>
-    <col min="5" max="5" width="13.69921875" customWidth="1"/>
-    <col min="6" max="27" width="7.59765625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="13.13"/>
+    <col customWidth="1" min="2" max="2" width="19.0"/>
+    <col customWidth="1" min="3" max="3" width="19.88"/>
+    <col customWidth="1" min="4" max="4" width="26.13"/>
+    <col customWidth="1" min="5" max="5" width="13.75"/>
+    <col customWidth="1" min="6" max="27" width="7.63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>6.11067085E8</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>611067085</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="F3" s="9">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1"/>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4378,7 +4421,9 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added "tick" and "cross" to dictionary. removed beneficiries dict, pending refactor
edited fields for client info excel sheet
edited templates
</commit_message>
<xml_diff>
--- a/src/input/00 Client information.xlsx
+++ b/src/input/00 Client information.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="588" yWindow="564" windowWidth="15996" windowHeight="5244"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Info" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Existing Insurance" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Beneficiaries" sheetId="3" r:id="rId6"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Existing Insurance" sheetId="2" r:id="rId2"/>
+    <sheet name="Beneficiaries" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t>No.</t>
   </si>
@@ -57,9 +60,6 @@
     <t>Chandni Gobind Samtani</t>
   </si>
   <si>
-    <t>self</t>
-  </si>
-  <si>
     <t>Client Information</t>
   </si>
   <si>
@@ -69,39 +69,9 @@
     <t>INSURED</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>OWNER</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -180,15 +150,6 @@
     <t>gib@eim.ae</t>
   </si>
   <si>
-    <t>HOME TEL</t>
-  </si>
-  <si>
-    <t>BUSSINESS TEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOBILE </t>
-  </si>
-  <si>
     <t>COUNTRY CODE</t>
   </si>
   <si>
@@ -228,9 +189,6 @@
     <t>RESIDENTIAL ADDRESS LINE 1</t>
   </si>
   <si>
-    <t>Villa-18/2A, 394/Emirates Hill, Third (Meadows-8), Premise Number 394041593, Dubai, UAE</t>
-  </si>
-  <si>
     <t>RESIDENTIAL ADDRESS LINE 2</t>
   </si>
   <si>
@@ -267,9 +225,6 @@
     <t>MARITAL STATUS</t>
   </si>
   <si>
-    <t xml:space="preserve">Maried </t>
-  </si>
-  <si>
     <t>Financial Info</t>
   </si>
   <si>
@@ -340,36 +295,77 @@
   </si>
   <si>
     <t>INVESTMENT VALUE (MUTUAL FUNDS / UNIT TRUSTS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Villa-18/2A, 394/Emirates Hill, Third (Meadows-8), </t>
+  </si>
+  <si>
+    <t>Premise Number 394041593, Dubai, UAE</t>
+  </si>
+  <si>
+    <t>TOLANI SANJAY</t>
+  </si>
+  <si>
+    <t>(SPOUSE)</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>553595566</t>
+  </si>
+  <si>
+    <t>971</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -377,7 +373,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -387,67 +383,50 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -637,653 +616,637 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z1024"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="41.75"/>
-    <col customWidth="1" min="2" max="2" width="67.63"/>
-    <col customWidth="1" min="3" max="3" width="8.5"/>
-    <col customWidth="1" min="4" max="4" width="32.5"/>
-    <col customWidth="1" min="5" max="5" width="9.0"/>
-    <col customWidth="1" min="6" max="6" width="11.25"/>
-    <col customWidth="1" min="7" max="26" width="7.63"/>
+    <col min="1" max="1" width="41.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" style="1" customWidth="1"/>
+    <col min="7" max="26" width="7.59765625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4">
-        <v>6.11067085E8</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="B1" s="3">
+        <v>611067085</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="7">
-        <v>5.53595566E8</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="7">
-        <v>971.0</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="7" t="s">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+    </row>
+    <row r="43" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A43" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="10" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="8" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A46" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A47" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="8" t="s">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="7" t="s">
+    </row>
+    <row r="48" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A48" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="10" t="s">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A49" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="10" t="s">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10" t="s">
+    </row>
+    <row r="50" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A50" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="10" t="s">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A51" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="10" t="s">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="10" t="s">
+    </row>
+    <row r="52" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A52" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="3" t="s">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="3" t="s">
+    </row>
+    <row r="54" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A54" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="3" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A55" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="3" t="s">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A56" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="3" t="s">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="3" t="s">
+    </row>
+    <row r="57" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A57" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A58" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="3" t="s">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A59" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2244,86 +2207,83 @@
     <row r="1022" ht="14.25" customHeight="1"/>
     <row r="1023" ht="14.25" customHeight="1"/>
     <row r="1024" ht="14.25" customHeight="1"/>
-    <row r="1025" ht="14.25" customHeight="1"/>
-    <row r="1026" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.5"/>
-    <col customWidth="1" min="2" max="2" width="16.25"/>
-    <col customWidth="1" min="3" max="3" width="8.38"/>
-    <col customWidth="1" min="4" max="4" width="4.38"/>
-    <col customWidth="1" min="5" max="5" width="8.88"/>
-    <col customWidth="1" min="6" max="6" width="11.13"/>
-    <col customWidth="1" min="7" max="7" width="10.13"/>
-    <col customWidth="1" min="8" max="26" width="7.63"/>
+    <col min="1" max="1" width="3.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.09765625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.09765625" style="8" customWidth="1"/>
+    <col min="8" max="26" width="7.59765625" style="8" customWidth="1"/>
+    <col min="27" max="16384" width="12.59765625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3309,132 +3269,88 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.13"/>
-    <col customWidth="1" min="2" max="2" width="19.0"/>
-    <col customWidth="1" min="3" max="3" width="19.88"/>
-    <col customWidth="1" min="4" max="4" width="26.13"/>
-    <col customWidth="1" min="5" max="5" width="13.75"/>
-    <col customWidth="1" min="6" max="27" width="7.63"/>
+    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.09765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" style="1" customWidth="1"/>
+    <col min="6" max="27" width="7.59765625" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="12.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2">
-        <v>6.11067085E8</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1">
+        <v>611067085</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:6" ht="13.8" customHeight="1">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4418,12 +4334,8 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added code to read templates from excel file. refactor setPDFData. changed the way beneficiaries data is stored.
</commit_message>
<xml_diff>
--- a/src/input/00 Client information.xlsx
+++ b/src/input/00 Client information.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Existing Insurance" sheetId="2" r:id="rId2"/>
-    <sheet name="Beneficiaries" sheetId="3" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="114">
   <si>
     <t>No.</t>
   </si>
@@ -27,9 +27,6 @@
     <t>OWNER OR INSURED</t>
   </si>
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
     <t>RELATIONSHIP TO SETTLOR</t>
   </si>
   <si>
@@ -51,12 +48,6 @@
     <t>RELATIONSHIP TO LIFE INSURED</t>
   </si>
   <si>
-    <t>ID/PASSPORT NO.</t>
-  </si>
-  <si>
-    <t>SHARE(%)</t>
-  </si>
-  <si>
     <t>Chandni Gobind Samtani</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>TITLE</t>
   </si>
   <si>
-    <t>Mrs.</t>
-  </si>
-  <si>
     <t>FAMILY NAME</t>
   </si>
   <si>
@@ -108,12 +96,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>HKID</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH (DD/MM/YY)</t>
-  </si>
-  <si>
     <t>13/06/1985</t>
   </si>
   <si>
@@ -126,24 +108,9 @@
     <t>NATIONALITY 2</t>
   </si>
   <si>
-    <t>TOWN/ CITY OF BIRTH</t>
-  </si>
-  <si>
     <t>COUNTRY OF BIRTH</t>
   </si>
   <si>
-    <t>TAX ID</t>
-  </si>
-  <si>
-    <t>US TAX ID</t>
-  </si>
-  <si>
-    <t>LOCAL TAX ID</t>
-  </si>
-  <si>
-    <t>COUNTRY OF LOCAL TAX ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">EMAIL </t>
   </si>
   <si>
@@ -162,30 +129,6 @@
     <t>OFFICE NUMBER</t>
   </si>
   <si>
-    <t>HOUSE/APT/SUITE/NUMBER/STREET</t>
-  </si>
-  <si>
-    <t>Villa-18/2A, 394/Emirates Hill, Third (Meadows-8), Premise Number 394041593</t>
-  </si>
-  <si>
-    <t>TOWN,CITY</t>
-  </si>
-  <si>
-    <t>Dubai</t>
-  </si>
-  <si>
-    <t>STATE/PROVINCE</t>
-  </si>
-  <si>
-    <t>COUNTRY</t>
-  </si>
-  <si>
-    <t>UAE</t>
-  </si>
-  <si>
-    <t>POSTEL CODE/ ZIP  CODE</t>
-  </si>
-  <si>
     <t>RESIDENTIAL ADDRESS LINE 1</t>
   </si>
   <si>
@@ -201,9 +144,6 @@
     <t>CORRESPONDENCE ADDRESS LINE 2</t>
   </si>
   <si>
-    <t>PREVIOUS ADDRESS</t>
-  </si>
-  <si>
     <t>HEIGHT</t>
   </si>
   <si>
@@ -225,9 +165,6 @@
     <t>MARITAL STATUS</t>
   </si>
   <si>
-    <t>Financial Info</t>
-  </si>
-  <si>
     <t>EMPLOYER NAME</t>
   </si>
   <si>
@@ -285,67 +222,153 @@
     <t>INVESTMENT EXPERIENCE</t>
   </si>
   <si>
-    <t>in stocks, bonds, mutual funds, unit trusts</t>
-  </si>
-  <si>
-    <t>INVESTMENT VALUE (STOCKS)</t>
-  </si>
-  <si>
-    <t>INVESTMENT VALUE (BONDS)</t>
-  </si>
-  <si>
-    <t>INVESTMENT VALUE (MUTUAL FUNDS / UNIT TRUSTS)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Villa-18/2A, 394/Emirates Hill, Third (Meadows-8), </t>
   </si>
   <si>
     <t>Premise Number 394041593, Dubai, UAE</t>
   </si>
   <si>
-    <t>TOLANI SANJAY</t>
-  </si>
-  <si>
-    <t>(SPOUSE)</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
     <t>Married</t>
   </si>
   <si>
-    <t>MOBILE</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>553595566</t>
   </si>
   <si>
     <t>971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATE OF BIRTH </t>
+  </si>
+  <si>
+    <t>(DD/MM/YY)</t>
+  </si>
+  <si>
+    <t>HKID OR PASSPORT</t>
+  </si>
+  <si>
+    <t>if different from NATIONALITY 1</t>
+  </si>
+  <si>
+    <t>MOBILE NUMBER</t>
+  </si>
+  <si>
+    <t>approximate investment value in USD</t>
+  </si>
+  <si>
+    <t>number of years</t>
+  </si>
+  <si>
+    <t>STOCKS</t>
+  </si>
+  <si>
+    <t>BONDS</t>
+  </si>
+  <si>
+    <t>MUTUAL FUNDS / UNIT TRUSTS</t>
+  </si>
+  <si>
+    <t>Financial Information</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>BENEFICIARY</t>
+  </si>
+  <si>
+    <t>SHARE (%)</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Tolani Sanjay</t>
+  </si>
+  <si>
+    <t>Sanjay</t>
+  </si>
+  <si>
+    <t>Tolani</t>
+  </si>
+  <si>
+    <t>only for beneficiary</t>
+  </si>
+  <si>
+    <t>Z4904967</t>
+  </si>
+  <si>
+    <t>ABU DHABI (UAE)</t>
+  </si>
+  <si>
+    <t>31/01/1983</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>43595566</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A B</t>
+  </si>
+  <si>
+    <t>A1234567</t>
+  </si>
+  <si>
+    <t>01/01/1991</t>
+  </si>
+  <si>
+    <t>SINGAPORE</t>
+  </si>
+  <si>
+    <t>MALAYSIA</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>97864744</t>
+  </si>
+  <si>
+    <t>abc@cde.com</t>
+  </si>
+  <si>
+    <t>405 Pasir Ris drive 6</t>
+  </si>
+  <si>
+    <t>#12-491, S510405</t>
+  </si>
+  <si>
+    <t>Rando</t>
+  </si>
+  <si>
+    <t>DATE OF BIRTH</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -361,14 +384,8 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +396,18 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -401,21 +430,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,25 +657,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1024"/>
+  <dimension ref="A1:Y1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.19921875" style="1" customWidth="1"/>
-    <col min="7" max="26" width="7.59765625" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="12.59765625" style="1"/>
+    <col min="1" max="1" width="28.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="40.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="25" width="7.59765625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="12.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" customHeight="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -649,604 +682,536 @@
         <v>611067085</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" customHeight="1">
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.25" customHeight="1">
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" s="8" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="C34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+    </row>
+    <row r="35" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A28" s="5" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A29" s="5" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="5" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A34" s="5" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:25" ht="14.25" customHeight="1">
+      <c r="A43" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A40" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-      <c r="X42" s="2"/>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-    </row>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1">
+    </row>
+    <row r="44" spans="1:25" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1">
+    </row>
+    <row r="45" spans="1:25" ht="14.25" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:26" ht="14.25" customHeight="1">
+    </row>
+    <row r="46" spans="1:25" ht="14.25" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1">
+    </row>
+    <row r="47" spans="1:25" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1">
+    </row>
+    <row r="48" spans="1:25" ht="14.25" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="14.25" customHeight="1">
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="14.25" customHeight="1">
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" ht="14.25" customHeight="1">
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A52" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A53" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A54" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A56" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A57" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A58" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A59" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:4" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2199,17 +2164,12 @@
     <row r="1014" ht="14.25" customHeight="1"/>
     <row r="1015" ht="14.25" customHeight="1"/>
     <row r="1016" ht="14.25" customHeight="1"/>
-    <row r="1017" ht="14.25" customHeight="1"/>
-    <row r="1018" ht="14.25" customHeight="1"/>
-    <row r="1019" ht="14.25" customHeight="1"/>
-    <row r="1020" ht="14.25" customHeight="1"/>
-    <row r="1021" ht="14.25" customHeight="1"/>
-    <row r="1022" ht="14.25" customHeight="1"/>
-    <row r="1023" ht="14.25" customHeight="1"/>
-    <row r="1024" ht="14.25" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E20" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2218,57 +2178,57 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="8.3984375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="4.3984375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.8984375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.09765625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="10.09765625" style="8" customWidth="1"/>
-    <col min="8" max="26" width="7.59765625" style="8" customWidth="1"/>
-    <col min="27" max="16384" width="12.59765625" style="8"/>
+    <col min="1" max="1" width="3.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.09765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.09765625" style="1" customWidth="1"/>
+    <col min="8" max="26" width="7.59765625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.59765625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A2" s="6">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
     </row>
@@ -3276,1066 +3236,349 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F999"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.09765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.69921875" style="1" customWidth="1"/>
-    <col min="6" max="27" width="7.59765625" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="12.59765625" style="1"/>
+    <col min="1" max="1" width="41.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>611067085</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.8" customHeight="1">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
+      <c r="B28" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>